<commit_message>
added booking and expedia folder inside working_windows_extension folder
</commit_message>
<xml_diff>
--- a/booking/Expenses.xlsx
+++ b/booking/Expenses.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>Confirmation Number</t>
   </si>
@@ -34,19 +34,34 @@
     <t>Fedrique PIERRE</t>
   </si>
   <si>
+    <t>242.97 USD</t>
+  </si>
+  <si>
     <t>Canceled</t>
   </si>
   <si>
     <t>Yaning Qiao</t>
   </si>
   <si>
+    <t>118.15 USD</t>
+  </si>
+  <si>
     <t>Checked in, but different date</t>
   </si>
   <si>
     <t>dongxu liu</t>
   </si>
   <si>
+    <t>95.45 USD</t>
+  </si>
+  <si>
     <t>Terrance Graham</t>
+  </si>
+  <si>
+    <t>119 USD</t>
+  </si>
+  <si>
+    <t>98.77 USD</t>
   </si>
 </sst>
 </file>
@@ -406,13 +421,16 @@
         <v>1877709056</v>
       </c>
       <c r="B2">
-        <v>59856768</v>
+        <v>59179638</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -423,10 +441,13 @@
         <v>72889558</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -437,10 +458,13 @@
         <v>81897220</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -448,13 +472,16 @@
         <v>1526364779</v>
       </c>
       <c r="B5">
-        <v>59856768</v>
+        <v>80862497</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -465,10 +492,13 @@
         <v>81424613</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>